<commit_message>
Atualização automática ARMAZÉM - 2025-11-06 16:25
</commit_message>
<xml_diff>
--- a/data/custo_pizzas.xlsx
+++ b/data/custo_pizzas.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19.25</v>
+        <v>17.69</v>
       </c>
       <c r="C2" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>50.65</v>
+        <v>52.21</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.7246065808297568</v>
+        <v>0.7469241773962805</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14.03</v>
+        <v>12.82</v>
       </c>
       <c r="C3" t="n">
         <v>59.9</v>
       </c>
       <c r="D3" t="n">
-        <v>45.87</v>
+        <v>47.08</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.7657762938230384</v>
+        <v>0.7859766277128547</v>
       </c>
     </row>
     <row r="4">
@@ -506,16 +506,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10.18</v>
+        <v>9.26</v>
       </c>
       <c r="C4" t="n">
         <v>49.9</v>
       </c>
       <c r="D4" t="n">
-        <v>39.72</v>
+        <v>40.64</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.7959919839679359</v>
+        <v>0.8144288577154309</v>
       </c>
     </row>
     <row r="5">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>15.88</v>
+        <v>14.32</v>
       </c>
       <c r="C5" t="n">
         <v>55.9</v>
       </c>
       <c r="D5" t="n">
-        <v>40.02</v>
+        <v>41.58</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.7159212880143112</v>
+        <v>0.7438282647584973</v>
       </c>
     </row>
     <row r="6">
@@ -544,16 +544,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11.63</v>
+        <v>10.51</v>
       </c>
       <c r="C6" t="n">
         <v>45.9</v>
       </c>
       <c r="D6" t="n">
-        <v>34.27</v>
+        <v>35.39</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.7466230936819171</v>
+        <v>0.7710239651416122</v>
       </c>
     </row>
     <row r="7">
@@ -563,16 +563,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8.5</v>
+        <v>7.69</v>
       </c>
       <c r="C7" t="n">
         <v>35.9</v>
       </c>
       <c r="D7" t="n">
-        <v>27.4</v>
+        <v>28.21</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.7632311977715878</v>
+        <v>0.7857938718662952</v>
       </c>
     </row>
     <row r="8">
@@ -582,16 +582,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12.78</v>
+        <v>11.23</v>
       </c>
       <c r="C8" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>57.12</v>
+        <v>58.67</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.8171673819742489</v>
+        <v>0.8393419170243204</v>
       </c>
     </row>
     <row r="9">
@@ -601,16 +601,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9.42</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="C9" t="n">
         <v>59.9</v>
       </c>
       <c r="D9" t="n">
-        <v>50.48</v>
+        <v>51.6</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.8427378964941569</v>
+        <v>0.8614357262103505</v>
       </c>
     </row>
     <row r="10">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6.86</v>
+        <v>6.05</v>
       </c>
       <c r="C10" t="n">
         <v>49.9</v>
       </c>
       <c r="D10" t="n">
-        <v>43.04</v>
+        <v>43.85</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.8625250501002004</v>
+        <v>0.8787575150300602</v>
       </c>
     </row>
     <row r="11">
@@ -639,16 +639,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>14</v>
+        <v>12.44</v>
       </c>
       <c r="C11" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>55.9</v>
+        <v>57.46</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.7997138769670958</v>
+        <v>0.8220314735336195</v>
       </c>
     </row>
     <row r="12">
@@ -658,16 +658,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10.27</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="C12" t="n">
         <v>59.9</v>
       </c>
       <c r="D12" t="n">
-        <v>49.63</v>
+        <v>50.76</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.8285475792988314</v>
+        <v>0.8474123539232054</v>
       </c>
     </row>
     <row r="13">
@@ -677,16 +677,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7.51</v>
+        <v>6.7</v>
       </c>
       <c r="C13" t="n">
         <v>49.9</v>
       </c>
       <c r="D13" t="n">
-        <v>42.39</v>
+        <v>43.2</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.849498997995992</v>
+        <v>0.8657314629258517</v>
       </c>
     </row>
     <row r="14">
@@ -696,16 +696,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>24.45</v>
+        <v>22.89</v>
       </c>
       <c r="C14" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D14" t="n">
-        <v>45.45</v>
+        <v>47.01</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0.6502145922746781</v>
+        <v>0.6725321888412017</v>
       </c>
     </row>
     <row r="15">
@@ -715,16 +715,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17.69</v>
+        <v>16.57</v>
       </c>
       <c r="C15" t="n">
         <v>59.9</v>
       </c>
       <c r="D15" t="n">
-        <v>42.21</v>
+        <v>43.33</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0.7046744574290483</v>
+        <v>0.723372287145242</v>
       </c>
     </row>
     <row r="16">
@@ -734,16 +734,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>12.73</v>
+        <v>11.92</v>
       </c>
       <c r="C16" t="n">
         <v>49.9</v>
       </c>
       <c r="D16" t="n">
-        <v>37.17</v>
+        <v>37.98</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0.7448897795591183</v>
+        <v>0.7611222444889779</v>
       </c>
     </row>
     <row r="17">
@@ -753,16 +753,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>22.03</v>
+        <v>20.47</v>
       </c>
       <c r="C17" t="n">
         <v>65.90000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>43.87</v>
+        <v>45.43</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0.6657056145675265</v>
+        <v>0.6893778452200304</v>
       </c>
     </row>
     <row r="18">
@@ -772,16 +772,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>15.95</v>
+        <v>14.82</v>
       </c>
       <c r="C18" t="n">
         <v>55.9</v>
       </c>
       <c r="D18" t="n">
-        <v>39.95</v>
+        <v>41.08</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0.7146690518783543</v>
+        <v>0.7348837209302326</v>
       </c>
     </row>
     <row r="19">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>11.48</v>
+        <v>10.67</v>
       </c>
       <c r="C19" t="n">
         <v>45.9</v>
       </c>
       <c r="D19" t="n">
-        <v>34.42</v>
+        <v>35.23</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.7498910675381264</v>
+        <v>0.7675381263616557</v>
       </c>
     </row>
     <row r="20">
@@ -810,16 +810,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>22.03</v>
+        <v>20.47</v>
       </c>
       <c r="C20" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>47.87</v>
+        <v>49.43</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.6848354792560801</v>
+        <v>0.7071530758226038</v>
       </c>
     </row>
     <row r="21">
@@ -829,16 +829,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>15.95</v>
+        <v>14.82</v>
       </c>
       <c r="C21" t="n">
         <v>59.9</v>
       </c>
       <c r="D21" t="n">
-        <v>43.95</v>
+        <v>45.08</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0.7337228714524208</v>
+        <v>0.7525876460767946</v>
       </c>
     </row>
     <row r="22">
@@ -848,16 +848,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>11.48</v>
+        <v>10.67</v>
       </c>
       <c r="C22" t="n">
         <v>49.9</v>
       </c>
       <c r="D22" t="n">
-        <v>38.42</v>
+        <v>39.23</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0.7699398797595191</v>
+        <v>0.7861723446893787</v>
       </c>
     </row>
     <row r="23">
@@ -867,16 +867,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>13.74</v>
+        <v>12.19</v>
       </c>
       <c r="C23" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>56.16</v>
+        <v>57.71</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.8034334763948497</v>
+        <v>0.8256080114449214</v>
       </c>
     </row>
     <row r="24">
@@ -886,16 +886,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>11.21</v>
+        <v>10.08</v>
       </c>
       <c r="C24" t="n">
         <v>59.9</v>
       </c>
       <c r="D24" t="n">
-        <v>48.69</v>
+        <v>49.82</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.8128547579298832</v>
+        <v>0.8317195325542571</v>
       </c>
     </row>
     <row r="25">
@@ -905,16 +905,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>8.06</v>
+        <v>7.25</v>
       </c>
       <c r="C25" t="n">
         <v>49.9</v>
       </c>
       <c r="D25" t="n">
-        <v>41.84</v>
+        <v>42.65</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.8384769539078156</v>
+        <v>0.8547094188376754</v>
       </c>
     </row>
     <row r="26">
@@ -924,16 +924,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>12.65</v>
+        <v>11.09</v>
       </c>
       <c r="C26" t="n">
         <v>65.90000000000001</v>
       </c>
       <c r="D26" t="n">
-        <v>53.25</v>
+        <v>54.81</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.8080424886191199</v>
+        <v>0.8317147192716237</v>
       </c>
     </row>
     <row r="27">
@@ -943,16 +943,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>9.17</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="C27" t="n">
         <v>55.9</v>
       </c>
       <c r="D27" t="n">
-        <v>46.73</v>
+        <v>47.85</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>0.8359570661896243</v>
+        <v>0.8559928443649373</v>
       </c>
     </row>
     <row r="28">
@@ -962,16 +962,16 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>6.6</v>
+        <v>5.79</v>
       </c>
       <c r="C28" t="n">
         <v>45.9</v>
       </c>
       <c r="D28" t="n">
-        <v>39.3</v>
+        <v>40.11</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>0.8562091503267973</v>
+        <v>0.8738562091503268</v>
       </c>
     </row>
     <row r="29">
@@ -981,16 +981,16 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>11.39</v>
+        <v>9.83</v>
       </c>
       <c r="C29" t="n">
         <v>45.9</v>
       </c>
       <c r="D29" t="n">
-        <v>34.51</v>
+        <v>36.07</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>0.7518518518518519</v>
+        <v>0.785838779956427</v>
       </c>
     </row>
     <row r="30">
@@ -1000,16 +1000,16 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>8.27</v>
+        <v>7.14</v>
       </c>
       <c r="C30" t="n">
         <v>37.9</v>
       </c>
       <c r="D30" t="n">
-        <v>29.63</v>
+        <v>30.76</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.7817941952506596</v>
+        <v>0.8116094986807387</v>
       </c>
     </row>
     <row r="31">
@@ -1019,16 +1019,16 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5.95</v>
+        <v>5.14</v>
       </c>
       <c r="C31" t="n">
         <v>32.9</v>
       </c>
       <c r="D31" t="n">
-        <v>26.95</v>
+        <v>27.76</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.8191489361702128</v>
+        <v>0.8437689969604864</v>
       </c>
     </row>
     <row r="32">
@@ -1064,7 +1064,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>5.9</v>
+        <v>5.54</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>0</v>
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>11.79</v>
+        <v>11.08</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>4.9</v>
+        <v>4.54</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>0</v>
@@ -1103,7 +1103,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>9.789999999999999</v>
+        <v>9.09</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
@@ -1135,16 +1135,16 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>5.71</v>
+        <v>5.7</v>
       </c>
       <c r="C39" t="n">
         <v>37.9</v>
       </c>
       <c r="D39" t="n">
-        <v>32.19</v>
+        <v>32.2</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>0.8493403693931398</v>
+        <v>0.8496042216358838</v>
       </c>
     </row>
     <row r="40">
@@ -1230,16 +1230,16 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>19.28</v>
+        <v>17.72</v>
       </c>
       <c r="C44" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D44" t="n">
-        <v>50.62</v>
+        <v>52.18</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>0.7241773962804006</v>
+        <v>0.7464949928469242</v>
       </c>
     </row>
     <row r="45">
@@ -1249,16 +1249,16 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>14.55</v>
+        <v>13.42</v>
       </c>
       <c r="C45" t="n">
         <v>59.9</v>
       </c>
       <c r="D45" t="n">
-        <v>45.35</v>
+        <v>46.48</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>0.7570951585976627</v>
+        <v>0.7759599332220367</v>
       </c>
     </row>
     <row r="46">
@@ -1268,16 +1268,16 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>10.46</v>
+        <v>9.65</v>
       </c>
       <c r="C46" t="n">
         <v>49.9</v>
       </c>
       <c r="D46" t="n">
-        <v>39.44</v>
+        <v>40.25</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>0.790380761523046</v>
+        <v>0.8066132264529058</v>
       </c>
     </row>
     <row r="47">
@@ -1287,16 +1287,16 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>15.9</v>
+        <v>14.34</v>
       </c>
       <c r="C47" t="n">
         <v>65.90000000000001</v>
       </c>
       <c r="D47" t="n">
-        <v>50</v>
+        <v>51.56</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>0.7587253414264037</v>
+        <v>0.7823975720789074</v>
       </c>
     </row>
     <row r="48">
@@ -1306,16 +1306,16 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>11.45</v>
+        <v>10.25</v>
       </c>
       <c r="C48" t="n">
         <v>55.9</v>
       </c>
       <c r="D48" t="n">
-        <v>44.45</v>
+        <v>45.65</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>0.7951699463327371</v>
+        <v>0.8166368515205724</v>
       </c>
     </row>
     <row r="49">
@@ -1325,16 +1325,16 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>8.98</v>
+        <v>8.06</v>
       </c>
       <c r="C49" t="n">
         <v>45.9</v>
       </c>
       <c r="D49" t="n">
-        <v>36.92</v>
+        <v>37.84</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>0.8043572984749456</v>
+        <v>0.824400871459695</v>
       </c>
     </row>
     <row r="50">
@@ -1344,16 +1344,16 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>13.54</v>
+        <v>11.95</v>
       </c>
       <c r="C50" t="n">
         <v>59.9</v>
       </c>
       <c r="D50" t="n">
-        <v>46.36</v>
+        <v>47.95</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>0.7739565943238731</v>
+        <v>0.8005008347245409</v>
       </c>
     </row>
     <row r="51">
@@ -1363,16 +1363,16 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>10.33</v>
+        <v>9.130000000000001</v>
       </c>
       <c r="C51" t="n">
         <v>49.9</v>
       </c>
       <c r="D51" t="n">
-        <v>39.57</v>
+        <v>40.77</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>0.7929859719438878</v>
+        <v>0.8170340681362724</v>
       </c>
     </row>
     <row r="52">
@@ -1382,16 +1382,16 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>8.48</v>
+        <v>7.56</v>
       </c>
       <c r="C52" t="n">
         <v>39.9</v>
       </c>
       <c r="D52" t="n">
-        <v>31.42</v>
+        <v>32.34</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>0.787468671679198</v>
+        <v>0.8105263157894737</v>
       </c>
     </row>
     <row r="53">
@@ -1401,16 +1401,16 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>19.02</v>
+        <v>17.46</v>
       </c>
       <c r="C53" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D53" t="n">
-        <v>50.88</v>
+        <v>52.44</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>0.7278969957081546</v>
+        <v>0.7502145922746781</v>
       </c>
     </row>
     <row r="54">
@@ -1420,16 +1420,16 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>13.77</v>
+        <v>12.65</v>
       </c>
       <c r="C54" t="n">
         <v>59.9</v>
       </c>
       <c r="D54" t="n">
-        <v>46.13</v>
+        <v>47.25</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>0.7701168614357261</v>
+        <v>0.7888146911519199</v>
       </c>
     </row>
     <row r="55">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>9.91</v>
+        <v>9.1</v>
       </c>
       <c r="C55" t="n">
         <v>49.9</v>
       </c>
       <c r="D55" t="n">
-        <v>39.99</v>
+        <v>40.8</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>0.8014028056112223</v>
+        <v>0.8176352705410821</v>
       </c>
     </row>
     <row r="56">
@@ -1458,16 +1458,16 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>14.48</v>
+        <v>14.12</v>
       </c>
       <c r="C56" t="n">
         <v>66.90000000000001</v>
       </c>
       <c r="D56" t="n">
-        <v>52.42</v>
+        <v>52.78</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>0.7835575485799701</v>
+        <v>0.7889387144992527</v>
       </c>
     </row>
     <row r="57">
@@ -1477,16 +1477,16 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>28.95</v>
+        <v>28.25</v>
       </c>
       <c r="C57" t="n">
         <v>95.90000000000001</v>
       </c>
       <c r="D57" t="n">
-        <v>66.95</v>
+        <v>67.65000000000001</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>0.6981230448383733</v>
+        <v>0.705422314911366</v>
       </c>
     </row>
     <row r="58">
@@ -1496,16 +1496,16 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>28.01</v>
+        <v>27.3</v>
       </c>
       <c r="C58" t="n">
         <v>79.90000000000001</v>
       </c>
       <c r="D58" t="n">
-        <v>51.89</v>
+        <v>52.6</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>0.6494367959949937</v>
+        <v>0.6583229036295369</v>
       </c>
     </row>
     <row r="59">
@@ -1515,16 +1515,16 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>40.89</v>
+        <v>40.18</v>
       </c>
       <c r="C59" t="n">
         <v>115.9</v>
       </c>
       <c r="D59" t="n">
-        <v>75.01000000000001</v>
+        <v>75.72</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>0.6471958584987058</v>
+        <v>0.6533218291630716</v>
       </c>
     </row>
     <row r="60">
@@ -1534,16 +1534,16 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>17.63</v>
+        <v>16.07</v>
       </c>
       <c r="C60" t="n">
         <v>79.90000000000001</v>
       </c>
       <c r="D60" t="n">
-        <v>62.27</v>
+        <v>63.83</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>0.7793491864831039</v>
+        <v>0.7988735919899875</v>
       </c>
     </row>
     <row r="61">
@@ -1553,16 +1553,16 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>12.77</v>
+        <v>11.64</v>
       </c>
       <c r="C61" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D61" t="n">
-        <v>57.13</v>
+        <v>58.26</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>0.817310443490701</v>
+        <v>0.8334763948497854</v>
       </c>
     </row>
     <row r="62">
@@ -1572,16 +1572,16 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>9.19</v>
+        <v>8.380000000000001</v>
       </c>
       <c r="C62" t="n">
         <v>59.9</v>
       </c>
       <c r="D62" t="n">
-        <v>50.71</v>
+        <v>51.52</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>0.8465776293823039</v>
+        <v>0.8601001669449081</v>
       </c>
     </row>
     <row r="63">
@@ -1591,16 +1591,16 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>18.27</v>
+        <v>16.72</v>
       </c>
       <c r="C63" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D63" t="n">
-        <v>51.63</v>
+        <v>53.18</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>0.7386266094420602</v>
+        <v>0.7608011444921317</v>
       </c>
     </row>
     <row r="64">
@@ -1610,16 +1610,16 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>11.81</v>
+        <v>10.68</v>
       </c>
       <c r="C64" t="n">
         <v>59.9</v>
       </c>
       <c r="D64" t="n">
-        <v>48.09</v>
+        <v>49.22</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>0.8028380634390651</v>
+        <v>0.821702838063439</v>
       </c>
     </row>
     <row r="65">
@@ -1629,16 +1629,16 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>8.5</v>
+        <v>7.69</v>
       </c>
       <c r="C65" t="n">
         <v>49.9</v>
       </c>
       <c r="D65" t="n">
-        <v>41.4</v>
+        <v>42.21</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>0.8296593186372745</v>
+        <v>0.8458917835671343</v>
       </c>
     </row>
     <row r="66">
@@ -1648,16 +1648,16 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>18.43</v>
+        <v>16.87</v>
       </c>
       <c r="C66" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D66" t="n">
-        <v>51.47</v>
+        <v>53.03</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>0.7363376251788269</v>
+        <v>0.7586552217453505</v>
       </c>
     </row>
     <row r="67">
@@ -1667,16 +1667,16 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>13.35</v>
+        <v>12.22</v>
       </c>
       <c r="C67" t="n">
         <v>59.9</v>
       </c>
       <c r="D67" t="n">
-        <v>46.55</v>
+        <v>47.68</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>0.7771285475792988</v>
+        <v>0.7959933222036728</v>
       </c>
     </row>
     <row r="68">
@@ -1686,16 +1686,16 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>9.609999999999999</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C68" t="n">
         <v>49.9</v>
       </c>
       <c r="D68" t="n">
-        <v>40.29</v>
+        <v>41.1</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>0.8074148296593187</v>
+        <v>0.8236472945891783</v>
       </c>
     </row>
     <row r="69">
@@ -1705,16 +1705,16 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>18.69</v>
+        <v>17.13</v>
       </c>
       <c r="C69" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D69" t="n">
-        <v>51.21</v>
+        <v>52.77</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>0.732618025751073</v>
+        <v>0.7549356223175967</v>
       </c>
     </row>
     <row r="70">
@@ -1724,16 +1724,16 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>13.54</v>
+        <v>12.41</v>
       </c>
       <c r="C70" t="n">
         <v>59.9</v>
       </c>
       <c r="D70" t="n">
-        <v>46.36</v>
+        <v>47.49</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>0.7739565943238731</v>
+        <v>0.7928213689482471</v>
       </c>
     </row>
     <row r="71">
@@ -1743,16 +1743,16 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>9.74</v>
+        <v>8.93</v>
       </c>
       <c r="C71" t="n">
         <v>49.9</v>
       </c>
       <c r="D71" t="n">
-        <v>40.16</v>
+        <v>40.97</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>0.8048096192384769</v>
+        <v>0.8210420841683367</v>
       </c>
     </row>
     <row r="72">
@@ -1762,16 +1762,16 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>18.29</v>
+        <v>16.74</v>
       </c>
       <c r="C72" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D72" t="n">
-        <v>51.61</v>
+        <v>53.16</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>0.7383404864091559</v>
+        <v>0.7605150214592276</v>
       </c>
     </row>
     <row r="73">
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>13.25</v>
+        <v>12.12</v>
       </c>
       <c r="C73" t="n">
         <v>59.9</v>
       </c>
       <c r="D73" t="n">
-        <v>46.65</v>
+        <v>47.78</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>0.7787979966611018</v>
+        <v>0.7976627712854758</v>
       </c>
     </row>
     <row r="74">
@@ -1800,16 +1800,16 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>9.539999999999999</v>
+        <v>8.73</v>
       </c>
       <c r="C74" t="n">
         <v>49.9</v>
       </c>
       <c r="D74" t="n">
-        <v>40.36</v>
+        <v>41.17</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>0.8088176352705411</v>
+        <v>0.8250501002004008</v>
       </c>
     </row>
     <row r="75">
@@ -1819,16 +1819,16 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>16.72</v>
+        <v>15.16</v>
       </c>
       <c r="C75" t="n">
         <v>65.90000000000001</v>
       </c>
       <c r="D75" t="n">
-        <v>49.18</v>
+        <v>50.74</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>0.7462822458270106</v>
+        <v>0.7699544764795145</v>
       </c>
     </row>
     <row r="76">
@@ -1838,16 +1838,16 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>12.23</v>
+        <v>11.03</v>
       </c>
       <c r="C76" t="n">
         <v>55.9</v>
       </c>
       <c r="D76" t="n">
-        <v>43.67</v>
+        <v>44.87</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>0.7812164579606441</v>
+        <v>0.8026833631484794</v>
       </c>
     </row>
     <row r="77">
@@ -1857,16 +1857,16 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>8.51</v>
+        <v>7.59</v>
       </c>
       <c r="C77" t="n">
         <v>45.9</v>
       </c>
       <c r="D77" t="n">
-        <v>37.39</v>
+        <v>38.31</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>0.8145969498910676</v>
+        <v>0.834640522875817</v>
       </c>
     </row>
     <row r="78">
@@ -1876,16 +1876,16 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>16.84</v>
+        <v>15.28</v>
       </c>
       <c r="C78" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D78" t="n">
-        <v>53.06</v>
+        <v>54.62</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>0.7590844062947067</v>
+        <v>0.7814020028612303</v>
       </c>
     </row>
     <row r="79">
@@ -1895,16 +1895,16 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>12.28</v>
+        <v>11.14</v>
       </c>
       <c r="C79" t="n">
         <v>59.9</v>
       </c>
       <c r="D79" t="n">
-        <v>47.62</v>
+        <v>48.76</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>0.7949916527545909</v>
+        <v>0.8140233722871453</v>
       </c>
     </row>
     <row r="80">
@@ -1914,16 +1914,16 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>8.85</v>
+        <v>8.02</v>
       </c>
       <c r="C80" t="n">
         <v>49.9</v>
       </c>
       <c r="D80" t="n">
-        <v>41.05</v>
+        <v>41.88</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>0.8226452905811623</v>
+        <v>0.8392785571142284</v>
       </c>
     </row>
     <row r="81">
@@ -1933,16 +1933,16 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>18.02</v>
+        <v>16.44</v>
       </c>
       <c r="C81" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D81" t="n">
-        <v>51.88</v>
+        <v>53.46</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>0.742203147353362</v>
+        <v>0.7648068669527898</v>
       </c>
     </row>
     <row r="82">
@@ -1952,16 +1952,16 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>13.05</v>
+        <v>11.91</v>
       </c>
       <c r="C82" t="n">
         <v>59.9</v>
       </c>
       <c r="D82" t="n">
-        <v>46.85</v>
+        <v>47.99</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>0.7821368948247077</v>
+        <v>0.8011686143572621</v>
       </c>
     </row>
     <row r="83">
@@ -1971,16 +1971,16 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>9.4</v>
+        <v>8.57</v>
       </c>
       <c r="C83" t="n">
         <v>49.9</v>
       </c>
       <c r="D83" t="n">
-        <v>40.5</v>
+        <v>41.33</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>0.811623246492986</v>
+        <v>0.8282565130260521</v>
       </c>
     </row>
     <row r="84">
@@ -1990,16 +1990,16 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>11.98</v>
+        <v>10.42</v>
       </c>
       <c r="C84" t="n">
         <v>55.9</v>
       </c>
       <c r="D84" t="n">
-        <v>43.92</v>
+        <v>45.48</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>0.7856887298747764</v>
+        <v>0.8135957066189624</v>
       </c>
     </row>
     <row r="85">
@@ -2009,16 +2009,16 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>8.69</v>
+        <v>7.57</v>
       </c>
       <c r="C85" t="n">
         <v>45.9</v>
       </c>
       <c r="D85" t="n">
-        <v>37.21</v>
+        <v>38.33</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>0.8106753812636166</v>
+        <v>0.8350762527233115</v>
       </c>
     </row>
     <row r="86">
@@ -2028,16 +2028,16 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>6.25</v>
+        <v>5.44</v>
       </c>
       <c r="C86" t="n">
         <v>35.9</v>
       </c>
       <c r="D86" t="n">
-        <v>29.65</v>
+        <v>30.46</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>0.8259052924791086</v>
+        <v>0.8484679665738161</v>
       </c>
     </row>
     <row r="87">
@@ -2047,16 +2047,16 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>13.24</v>
+        <v>11.69</v>
       </c>
       <c r="C87" t="n">
         <v>56.9</v>
       </c>
       <c r="D87" t="n">
-        <v>43.66</v>
+        <v>45.21</v>
       </c>
       <c r="E87" s="2" t="n">
-        <v>0.7673110720562389</v>
+        <v>0.7945518453427065</v>
       </c>
     </row>
     <row r="88">
@@ -2066,16 +2066,16 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>9.609999999999999</v>
+        <v>8.48</v>
       </c>
       <c r="C88" t="n">
         <v>55.9</v>
       </c>
       <c r="D88" t="n">
-        <v>46.29</v>
+        <v>47.42</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>0.8280858676207513</v>
+        <v>0.8483005366726297</v>
       </c>
     </row>
     <row r="89">
@@ -2085,16 +2085,16 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>6.91</v>
+        <v>6.1</v>
       </c>
       <c r="C89" t="n">
         <v>45.9</v>
       </c>
       <c r="D89" t="n">
-        <v>38.99</v>
+        <v>39.8</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>0.8494553376906318</v>
+        <v>0.8671023965141612</v>
       </c>
     </row>
     <row r="90">
@@ -2104,16 +2104,16 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>18.04</v>
+        <v>16.48</v>
       </c>
       <c r="C90" t="n">
         <v>68.90000000000001</v>
       </c>
       <c r="D90" t="n">
-        <v>50.86</v>
+        <v>52.42</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>0.7381712626995646</v>
+        <v>0.7608127721335268</v>
       </c>
     </row>
     <row r="91">
@@ -2123,16 +2123,16 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>11.33</v>
+        <v>10.21</v>
       </c>
       <c r="C91" t="n">
         <v>58.9</v>
       </c>
       <c r="D91" t="n">
-        <v>47.57</v>
+        <v>48.69</v>
       </c>
       <c r="E91" s="2" t="n">
-        <v>0.8076400679117148</v>
+        <v>0.8266553480475382</v>
       </c>
     </row>
     <row r="92">
@@ -2142,16 +2142,16 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>8.16</v>
+        <v>7.35</v>
       </c>
       <c r="C92" t="n">
         <v>48.9</v>
       </c>
       <c r="D92" t="n">
-        <v>40.74</v>
+        <v>41.55</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>0.8331288343558282</v>
+        <v>0.8496932515337423</v>
       </c>
     </row>
     <row r="93">
@@ -2161,16 +2161,16 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>16.53</v>
+        <v>14.97</v>
       </c>
       <c r="C93" t="n">
         <v>55.9</v>
       </c>
       <c r="D93" t="n">
-        <v>39.37</v>
+        <v>40.93</v>
       </c>
       <c r="E93" s="2" t="n">
-        <v>0.704293381037567</v>
+        <v>0.7322003577817532</v>
       </c>
     </row>
     <row r="94">
@@ -2180,16 +2180,16 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>11.98</v>
+        <v>10.85</v>
       </c>
       <c r="C94" t="n">
         <v>45.9</v>
       </c>
       <c r="D94" t="n">
-        <v>33.92</v>
+        <v>35.05</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>0.7389978213507626</v>
+        <v>0.7636165577342048</v>
       </c>
     </row>
     <row r="95">
@@ -2199,16 +2199,16 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>8.619999999999999</v>
+        <v>7.81</v>
       </c>
       <c r="C95" t="n">
         <v>35.9</v>
       </c>
       <c r="D95" t="n">
-        <v>27.28</v>
+        <v>28.09</v>
       </c>
       <c r="E95" s="2" t="n">
-        <v>0.7598885793871867</v>
+        <v>0.7824512534818941</v>
       </c>
     </row>
     <row r="96">
@@ -2218,16 +2218,16 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>11.98</v>
+        <v>10.42</v>
       </c>
       <c r="C96" t="n">
         <v>55.9</v>
       </c>
       <c r="D96" t="n">
-        <v>43.92</v>
+        <v>45.48</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>0.7856887298747764</v>
+        <v>0.8135957066189624</v>
       </c>
     </row>
     <row r="97">
@@ -2237,16 +2237,16 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>8.69</v>
+        <v>7.57</v>
       </c>
       <c r="C97" t="n">
         <v>45.9</v>
       </c>
       <c r="D97" t="n">
-        <v>37.21</v>
+        <v>38.33</v>
       </c>
       <c r="E97" s="2" t="n">
-        <v>0.8106753812636166</v>
+        <v>0.8350762527233115</v>
       </c>
     </row>
     <row r="98">
@@ -2256,16 +2256,16 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>6.25</v>
+        <v>5.44</v>
       </c>
       <c r="C98" t="n">
         <v>35.9</v>
       </c>
       <c r="D98" t="n">
-        <v>29.65</v>
+        <v>30.46</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>0.8259052924791086</v>
+        <v>0.8484679665738161</v>
       </c>
     </row>
     <row r="99">
@@ -2275,16 +2275,16 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>16.37</v>
+        <v>14.82</v>
       </c>
       <c r="C99" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D99" t="n">
-        <v>53.53</v>
+        <v>55.08</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>0.7658082975679542</v>
+        <v>0.7879828326180258</v>
       </c>
     </row>
     <row r="100">
@@ -2294,16 +2294,16 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>11.86</v>
+        <v>10.74</v>
       </c>
       <c r="C100" t="n">
         <v>59.9</v>
       </c>
       <c r="D100" t="n">
-        <v>48.04</v>
+        <v>49.16</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>0.8020033388981637</v>
+        <v>0.8207011686143573</v>
       </c>
     </row>
     <row r="101">
@@ -2313,16 +2313,16 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>8.539999999999999</v>
+        <v>7.73</v>
       </c>
       <c r="C101" t="n">
         <v>49.9</v>
       </c>
       <c r="D101" t="n">
-        <v>41.36</v>
+        <v>42.17</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>0.8288577154308617</v>
+        <v>0.8450901803607215</v>
       </c>
     </row>
     <row r="102">
@@ -2332,16 +2332,16 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>19.18</v>
+        <v>17.63</v>
       </c>
       <c r="C102" t="n">
         <v>65.90000000000001</v>
       </c>
       <c r="D102" t="n">
-        <v>46.72</v>
+        <v>48.27</v>
       </c>
       <c r="E102" s="2" t="n">
-        <v>0.7089529590288316</v>
+        <v>0.7324734446130502</v>
       </c>
     </row>
     <row r="103">
@@ -2351,16 +2351,16 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>13.89</v>
+        <v>12.77</v>
       </c>
       <c r="C103" t="n">
         <v>55.9</v>
       </c>
       <c r="D103" t="n">
-        <v>42.01</v>
+        <v>43.13</v>
       </c>
       <c r="E103" s="2" t="n">
-        <v>0.7515205724508049</v>
+        <v>0.771556350626118</v>
       </c>
     </row>
     <row r="104">
@@ -2370,16 +2370,16 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>10</v>
+        <v>9.19</v>
       </c>
       <c r="C104" t="n">
         <v>45.9</v>
       </c>
       <c r="D104" t="n">
-        <v>35.9</v>
+        <v>36.71</v>
       </c>
       <c r="E104" s="2" t="n">
-        <v>0.7821350762527233</v>
+        <v>0.7997821350762527</v>
       </c>
     </row>
     <row r="105">
@@ -2389,16 +2389,16 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>8.34</v>
+        <v>7.84</v>
       </c>
       <c r="C105" t="n">
         <v>45.9</v>
       </c>
       <c r="D105" t="n">
-        <v>37.56</v>
+        <v>38.06</v>
       </c>
       <c r="E105" s="2" t="n">
-        <v>0.8183006535947713</v>
+        <v>0.8291938997821352</v>
       </c>
     </row>
     <row r="106">
@@ -2408,16 +2408,16 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>6.21</v>
+        <v>5.7</v>
       </c>
       <c r="C106" t="n">
         <v>37.9</v>
       </c>
       <c r="D106" t="n">
-        <v>31.69</v>
+        <v>32.2</v>
       </c>
       <c r="E106" s="2" t="n">
-        <v>0.8361477572559366</v>
+        <v>0.8496042216358838</v>
       </c>
     </row>
     <row r="107">
@@ -2427,16 +2427,16 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>4.6</v>
+        <v>4.1</v>
       </c>
       <c r="C107" t="n">
         <v>32.9</v>
       </c>
       <c r="D107" t="n">
-        <v>28.3</v>
+        <v>28.8</v>
       </c>
       <c r="E107" s="2" t="n">
-        <v>0.8601823708206686</v>
+        <v>0.8753799392097263</v>
       </c>
     </row>
     <row r="108">
@@ -2446,16 +2446,16 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>17.88</v>
+        <v>17.17</v>
       </c>
       <c r="C108" t="n">
         <v>79.90000000000001</v>
       </c>
       <c r="D108" t="n">
-        <v>62.02</v>
+        <v>62.73</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>0.7762202753441803</v>
+        <v>0.7851063829787234</v>
       </c>
     </row>
     <row r="109">
@@ -2465,16 +2465,16 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>32.55</v>
+        <v>31.85</v>
       </c>
       <c r="C109" t="n">
         <v>115.9</v>
       </c>
       <c r="D109" t="n">
-        <v>83.34999999999999</v>
+        <v>84.05</v>
       </c>
       <c r="E109" s="2" t="n">
-        <v>0.7191544434857636</v>
+        <v>0.7251941328731666</v>
       </c>
     </row>
     <row r="110">
@@ -2484,16 +2484,16 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>29.81</v>
+        <v>29.1</v>
       </c>
       <c r="C110" t="n">
         <v>89.90000000000001</v>
       </c>
       <c r="D110" t="n">
-        <v>60.09</v>
+        <v>60.8</v>
       </c>
       <c r="E110" s="2" t="n">
-        <v>0.6684093437152392</v>
+        <v>0.6763070077864294</v>
       </c>
     </row>
     <row r="111">
@@ -2503,16 +2503,16 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>44.49</v>
+        <v>43.78</v>
       </c>
       <c r="C111" t="n">
         <v>129.9</v>
       </c>
       <c r="D111" t="n">
-        <v>85.41</v>
+        <v>86.12</v>
       </c>
       <c r="E111" s="2" t="n">
-        <v>0.6575057736720554</v>
+        <v>0.6629715165511932</v>
       </c>
     </row>
     <row r="112">
@@ -2522,16 +2522,16 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>22.81</v>
+        <v>21.25</v>
       </c>
       <c r="C112" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D112" t="n">
-        <v>47.09</v>
+        <v>48.65</v>
       </c>
       <c r="E112" s="2" t="n">
-        <v>0.6736766809728183</v>
+        <v>0.695994277539342</v>
       </c>
     </row>
     <row r="113">
@@ -2541,16 +2541,16 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>16.51</v>
+        <v>15.39</v>
       </c>
       <c r="C113" t="n">
         <v>59.9</v>
       </c>
       <c r="D113" t="n">
-        <v>43.39</v>
+        <v>44.51</v>
       </c>
       <c r="E113" s="2" t="n">
-        <v>0.7243739565943239</v>
+        <v>0.7430717863105175</v>
       </c>
     </row>
     <row r="114">
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>11.89</v>
+        <v>11.08</v>
       </c>
       <c r="C114" t="n">
         <v>49.9</v>
       </c>
       <c r="D114" t="n">
-        <v>38.01</v>
+        <v>38.82</v>
       </c>
       <c r="E114" s="2" t="n">
-        <v>0.7617234468937876</v>
+        <v>0.7779559118236473</v>
       </c>
     </row>
     <row r="115">
@@ -2579,16 +2579,16 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>15.73</v>
+        <v>14.18</v>
       </c>
       <c r="C115" t="n">
         <v>65.90000000000001</v>
       </c>
       <c r="D115" t="n">
-        <v>50.17</v>
+        <v>51.72</v>
       </c>
       <c r="E115" s="2" t="n">
-        <v>0.7613050075872534</v>
+        <v>0.784825493171472</v>
       </c>
     </row>
     <row r="116">
@@ -2598,16 +2598,16 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>11.64</v>
+        <v>10.51</v>
       </c>
       <c r="C116" t="n">
         <v>55.9</v>
       </c>
       <c r="D116" t="n">
-        <v>44.26</v>
+        <v>45.39</v>
       </c>
       <c r="E116" s="2" t="n">
-        <v>0.7917710196779965</v>
+        <v>0.8119856887298748</v>
       </c>
     </row>
     <row r="117">
@@ -2617,16 +2617,16 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>8.609999999999999</v>
+        <v>7.8</v>
       </c>
       <c r="C117" t="n">
         <v>45.9</v>
       </c>
       <c r="D117" t="n">
-        <v>37.29</v>
+        <v>38.1</v>
       </c>
       <c r="E117" s="2" t="n">
-        <v>0.8124183006535948</v>
+        <v>0.8300653594771242</v>
       </c>
     </row>
     <row r="118">
@@ -2636,16 +2636,16 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>18.48</v>
+        <v>16.92</v>
       </c>
       <c r="C118" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D118" t="n">
-        <v>51.42</v>
+        <v>52.98</v>
       </c>
       <c r="E118" s="2" t="n">
-        <v>0.7356223175965665</v>
+        <v>0.7579399141630901</v>
       </c>
     </row>
     <row r="119">
@@ -2655,16 +2655,16 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>13.62</v>
+        <v>12.49</v>
       </c>
       <c r="C119" t="n">
         <v>59.9</v>
       </c>
       <c r="D119" t="n">
-        <v>46.28</v>
+        <v>47.41</v>
       </c>
       <c r="E119" s="2" t="n">
-        <v>0.7726210350584307</v>
+        <v>0.7914858096828047</v>
       </c>
     </row>
     <row r="120">
@@ -2674,16 +2674,16 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>10.04</v>
+        <v>9.23</v>
       </c>
       <c r="C120" t="n">
         <v>49.9</v>
       </c>
       <c r="D120" t="n">
-        <v>39.86</v>
+        <v>40.67</v>
       </c>
       <c r="E120" s="2" t="n">
-        <v>0.7987975951903807</v>
+        <v>0.8150300601202405</v>
       </c>
     </row>
     <row r="121">
@@ -2712,16 +2712,16 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>8.279999999999999</v>
+        <v>8.27</v>
       </c>
       <c r="C122" t="n">
         <v>37.9</v>
       </c>
       <c r="D122" t="n">
-        <v>29.62</v>
+        <v>29.63</v>
       </c>
       <c r="E122" s="2" t="n">
-        <v>0.7815303430079156</v>
+        <v>0.7817941952506596</v>
       </c>
     </row>
     <row r="123">
@@ -2750,16 +2750,16 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>13.96</v>
+        <v>12.4</v>
       </c>
       <c r="C124" t="n">
         <v>65.90000000000001</v>
       </c>
       <c r="D124" t="n">
-        <v>51.94</v>
+        <v>53.5</v>
       </c>
       <c r="E124" s="2" t="n">
-        <v>0.7881638846737481</v>
+        <v>0.8118361153262519</v>
       </c>
     </row>
     <row r="125">
@@ -2769,16 +2769,16 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>10.12</v>
+        <v>9</v>
       </c>
       <c r="C125" t="n">
         <v>55.9</v>
       </c>
       <c r="D125" t="n">
-        <v>45.78</v>
+        <v>46.9</v>
       </c>
       <c r="E125" s="2" t="n">
-        <v>0.8189624329159213</v>
+        <v>0.8389982110912343</v>
       </c>
     </row>
     <row r="126">
@@ -2788,16 +2788,16 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>7.28</v>
+        <v>6.47</v>
       </c>
       <c r="C126" t="n">
         <v>45.9</v>
       </c>
       <c r="D126" t="n">
-        <v>38.62</v>
+        <v>39.43</v>
       </c>
       <c r="E126" s="2" t="n">
-        <v>0.8413943355119825</v>
+        <v>0.859041394335512</v>
       </c>
     </row>
     <row r="127">
@@ -2807,16 +2807,16 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>17.49</v>
+        <v>15.93</v>
       </c>
       <c r="C127" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D127" t="n">
-        <v>52.41</v>
+        <v>53.97</v>
       </c>
       <c r="E127" s="2" t="n">
-        <v>0.749785407725322</v>
+        <v>0.7721030042918455</v>
       </c>
     </row>
     <row r="128">
@@ -2826,16 +2826,16 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>12.67</v>
+        <v>11.55</v>
       </c>
       <c r="C128" t="n">
         <v>59.9</v>
       </c>
       <c r="D128" t="n">
-        <v>47.23</v>
+        <v>48.35</v>
       </c>
       <c r="E128" s="2" t="n">
-        <v>0.7884808013355592</v>
+        <v>0.8071786310517528</v>
       </c>
     </row>
     <row r="129">
@@ -2845,16 +2845,16 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>9.119999999999999</v>
+        <v>8.31</v>
       </c>
       <c r="C129" t="n">
         <v>49.9</v>
       </c>
       <c r="D129" t="n">
-        <v>40.78</v>
+        <v>41.59</v>
       </c>
       <c r="E129" s="2" t="n">
-        <v>0.8172344689378758</v>
+        <v>0.8334669338677354</v>
       </c>
     </row>
     <row r="130">
@@ -2864,16 +2864,16 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>16.42</v>
+        <v>14.86</v>
       </c>
       <c r="C130" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D130" t="n">
-        <v>53.48</v>
+        <v>55.04</v>
       </c>
       <c r="E130" s="2" t="n">
-        <v>0.7650929899856939</v>
+        <v>0.7874105865522175</v>
       </c>
     </row>
     <row r="131">
@@ -2883,16 +2883,16 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>11.9</v>
+        <v>10.77</v>
       </c>
       <c r="C131" t="n">
         <v>59.9</v>
       </c>
       <c r="D131" t="n">
-        <v>48</v>
+        <v>49.13</v>
       </c>
       <c r="E131" s="2" t="n">
-        <v>0.8013355592654424</v>
+        <v>0.8202003338898163</v>
       </c>
     </row>
     <row r="132">
@@ -2902,16 +2902,16 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>8.56</v>
+        <v>7.75</v>
       </c>
       <c r="C132" t="n">
         <v>49.9</v>
       </c>
       <c r="D132" t="n">
-        <v>41.34</v>
+        <v>42.15</v>
       </c>
       <c r="E132" s="2" t="n">
-        <v>0.8284569138276553</v>
+        <v>0.844689378757515</v>
       </c>
     </row>
     <row r="133">
@@ -2921,16 +2921,16 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>19.79</v>
+        <v>18.23</v>
       </c>
       <c r="C133" t="n">
         <v>69.90000000000001</v>
       </c>
       <c r="D133" t="n">
-        <v>50.11</v>
+        <v>51.67</v>
       </c>
       <c r="E133" s="2" t="n">
-        <v>0.7168812589413448</v>
+        <v>0.7391988555078683</v>
       </c>
     </row>
     <row r="134">
@@ -2940,16 +2940,16 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>14.33</v>
+        <v>13.2</v>
       </c>
       <c r="C134" t="n">
         <v>59.9</v>
       </c>
       <c r="D134" t="n">
-        <v>45.57</v>
+        <v>46.7</v>
       </c>
       <c r="E134" s="2" t="n">
-        <v>0.7607679465776294</v>
+        <v>0.7796327212020034</v>
       </c>
     </row>
     <row r="135">
@@ -2959,16 +2959,16 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>10.31</v>
+        <v>9.5</v>
       </c>
       <c r="C135" t="n">
         <v>49.9</v>
       </c>
       <c r="D135" t="n">
-        <v>39.59</v>
+        <v>40.4</v>
       </c>
       <c r="E135" s="2" t="n">
-        <v>0.7933867735470941</v>
+        <v>0.8096192384769539</v>
       </c>
     </row>
     <row r="136">
@@ -3073,16 +3073,16 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>16.37</v>
+        <v>14.81</v>
       </c>
       <c r="C141" t="n">
         <v>68.90000000000001</v>
       </c>
       <c r="D141" t="n">
-        <v>52.53</v>
+        <v>54.09</v>
       </c>
       <c r="E141" s="2" t="n">
-        <v>0.7624092888243831</v>
+        <v>0.7850507982583455</v>
       </c>
     </row>
     <row r="142">
@@ -3092,16 +3092,16 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>11.86</v>
+        <v>10.74</v>
       </c>
       <c r="C142" t="n">
         <v>58.9</v>
       </c>
       <c r="D142" t="n">
-        <v>47.04</v>
+        <v>48.16</v>
       </c>
       <c r="E142" s="2" t="n">
-        <v>0.798641765704584</v>
+        <v>0.8176570458404074</v>
       </c>
     </row>
     <row r="143">
@@ -3111,16 +3111,16 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>8.539999999999999</v>
+        <v>7.73</v>
       </c>
       <c r="C143" t="n">
         <v>48.9</v>
       </c>
       <c r="D143" t="n">
-        <v>40.36</v>
+        <v>41.17</v>
       </c>
       <c r="E143" s="2" t="n">
-        <v>0.8253578732106339</v>
+        <v>0.8419222903885482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>